<commit_message>
found typo in BDEQ
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BDEQ/BAU Distribued Electricity Quantities.xlsx
+++ b/InputData/bldgs/BDEQ/BAU Distribued Electricity Quantities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\US_EPS\InputData\bldgs\BDEQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC140EA-BD28-47AA-9020-848F7A9FCC62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91592BB-B4D9-4B36-B1D7-6E2ACBA7898C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="585" windowWidth="27000" windowHeight="14670" firstSheet="9" activeTab="10" xr2:uid="{EAFC2935-000E-413A-B5D2-814429F7674A}"/>
+    <workbookView xWindow="5850" yWindow="345" windowWidth="21870" windowHeight="14505" firstSheet="4" activeTab="4" xr2:uid="{EAFC2935-000E-413A-B5D2-814429F7674A}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2924,6 +2924,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2942,7 +2943,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="6" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="52">
     <cellStyle name="20% - Accent1" xfId="28" builtinId="30" customBuiltin="1"/>
@@ -7580,7 +7580,7 @@
                 <c:formatCode>0.000E+00</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -33423,7 +33423,7 @@
   </sheetPr>
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -35669,14 +35669,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4B961F-E56E-4DFD-B45A-CF05FF85A12C}">
   <dimension ref="A1:AK93"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" style="50" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" style="44" customWidth="1"/>
     <col min="3" max="3" width="35.5703125" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" customWidth="1"/>
   </cols>
@@ -35702,7 +35702,7 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="44" t="s">
         <v>235</v>
       </c>
       <c r="C5" t="s">
@@ -35831,7 +35831,7 @@
       <c r="A8" t="s">
         <v>239</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="44" t="s">
         <v>240</v>
       </c>
       <c r="C8" t="s">
@@ -35941,7 +35941,7 @@
       <c r="A9" t="s">
         <v>242</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="44" t="s">
         <v>243</v>
       </c>
       <c r="C9" t="s">
@@ -36051,7 +36051,7 @@
       <c r="A10" t="s">
         <v>244</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="44" t="s">
         <v>245</v>
       </c>
       <c r="C10" t="s">
@@ -36161,7 +36161,7 @@
       <c r="A11" t="s">
         <v>246</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="44" t="s">
         <v>247</v>
       </c>
       <c r="C11" t="s">
@@ -36271,7 +36271,7 @@
       <c r="A12" t="s">
         <v>248</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="44" t="s">
         <v>249</v>
       </c>
       <c r="C12" t="s">
@@ -36381,7 +36381,7 @@
       <c r="A13" t="s">
         <v>192</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="44" t="s">
         <v>250</v>
       </c>
       <c r="C13" t="s">
@@ -36491,7 +36491,7 @@
       <c r="A14" t="s">
         <v>251</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="44" t="s">
         <v>252</v>
       </c>
       <c r="C14" t="s">
@@ -36601,7 +36601,7 @@
       <c r="A15" t="s">
         <v>253</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="44" t="s">
         <v>254</v>
       </c>
       <c r="C15" t="s">
@@ -36711,7 +36711,7 @@
       <c r="A16" t="s">
         <v>255</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="44" t="s">
         <v>256</v>
       </c>
       <c r="C16" t="s">
@@ -36821,7 +36821,7 @@
       <c r="A17" t="s">
         <v>257</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="44" t="s">
         <v>258</v>
       </c>
       <c r="C17" t="s">
@@ -36939,7 +36939,7 @@
       <c r="A19" t="s">
         <v>239</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="44" t="s">
         <v>260</v>
       </c>
       <c r="C19" t="s">
@@ -37049,7 +37049,7 @@
       <c r="A20" t="s">
         <v>244</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="44" t="s">
         <v>261</v>
       </c>
       <c r="C20" t="s">
@@ -37159,7 +37159,7 @@
       <c r="A21" t="s">
         <v>255</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="44" t="s">
         <v>262</v>
       </c>
       <c r="C21" t="s">
@@ -37269,7 +37269,7 @@
       <c r="A22" t="s">
         <v>263</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="44" t="s">
         <v>264</v>
       </c>
       <c r="C22" t="s">
@@ -37379,7 +37379,7 @@
       <c r="A23" t="s">
         <v>265</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="44" t="s">
         <v>266</v>
       </c>
       <c r="C23" t="s">
@@ -37489,7 +37489,7 @@
       <c r="A24" t="s">
         <v>257</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="44" t="s">
         <v>267</v>
       </c>
       <c r="C24" t="s">
@@ -37607,7 +37607,7 @@
       <c r="A26" t="s">
         <v>269</v>
       </c>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="44" t="s">
         <v>270</v>
       </c>
       <c r="C26" t="s">
@@ -37717,7 +37717,7 @@
       <c r="A27" t="s">
         <v>271</v>
       </c>
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="44" t="s">
         <v>272</v>
       </c>
       <c r="C27" t="s">
@@ -37827,7 +37827,7 @@
       <c r="A28" t="s">
         <v>248</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="44" t="s">
         <v>273</v>
       </c>
       <c r="C28" t="s">
@@ -37937,7 +37937,7 @@
       <c r="A29" t="s">
         <v>192</v>
       </c>
-      <c r="B29" s="50" t="s">
+      <c r="B29" s="44" t="s">
         <v>274</v>
       </c>
       <c r="C29" t="s">
@@ -38047,7 +38047,7 @@
       <c r="A30" t="s">
         <v>275</v>
       </c>
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="44" t="s">
         <v>276</v>
       </c>
       <c r="C30" t="s">
@@ -38157,7 +38157,7 @@
       <c r="A31" t="s">
         <v>257</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="44" t="s">
         <v>277</v>
       </c>
       <c r="C31" t="s">
@@ -38275,7 +38275,7 @@
       <c r="A33" t="s">
         <v>269</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="44" t="s">
         <v>279</v>
       </c>
       <c r="C33" t="s">
@@ -38385,7 +38385,7 @@
       <c r="A34" t="s">
         <v>271</v>
       </c>
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="44" t="s">
         <v>280</v>
       </c>
       <c r="C34" t="s">
@@ -38495,7 +38495,7 @@
       <c r="A35" t="s">
         <v>192</v>
       </c>
-      <c r="B35" s="50" t="s">
+      <c r="B35" s="44" t="s">
         <v>281</v>
       </c>
       <c r="C35" t="s">
@@ -38605,7 +38605,7 @@
       <c r="A36" t="s">
         <v>257</v>
       </c>
-      <c r="B36" s="50" t="s">
+      <c r="B36" s="44" t="s">
         <v>282</v>
       </c>
       <c r="C36" t="s">
@@ -38723,7 +38723,7 @@
       <c r="A38" t="s">
         <v>269</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="44" t="s">
         <v>284</v>
       </c>
       <c r="C38" t="s">
@@ -38833,7 +38833,7 @@
       <c r="A39" t="s">
         <v>271</v>
       </c>
-      <c r="B39" s="50" t="s">
+      <c r="B39" s="44" t="s">
         <v>285</v>
       </c>
       <c r="C39" t="s">
@@ -38943,7 +38943,7 @@
       <c r="A40" t="s">
         <v>257</v>
       </c>
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="44" t="s">
         <v>286</v>
       </c>
       <c r="C40" t="s">
@@ -39061,7 +39061,7 @@
       <c r="A42" t="s">
         <v>288</v>
       </c>
-      <c r="B42" s="50" t="s">
+      <c r="B42" s="44" t="s">
         <v>289</v>
       </c>
       <c r="C42" t="s">
@@ -39171,7 +39171,7 @@
       <c r="A43" t="s">
         <v>290</v>
       </c>
-      <c r="B43" s="50" t="s">
+      <c r="B43" s="44" t="s">
         <v>291</v>
       </c>
       <c r="C43" t="s">
@@ -39297,7 +39297,7 @@
       <c r="A46" t="s">
         <v>292</v>
       </c>
-      <c r="B46" s="50" t="s">
+      <c r="B46" s="44" t="s">
         <v>293</v>
       </c>
       <c r="C46" t="s">
@@ -39407,7 +39407,7 @@
       <c r="A47" t="s">
         <v>295</v>
       </c>
-      <c r="B47" s="50" t="s">
+      <c r="B47" s="44" t="s">
         <v>296</v>
       </c>
       <c r="C47" t="s">
@@ -39517,7 +39517,7 @@
       <c r="A48" t="s">
         <v>298</v>
       </c>
-      <c r="B48" s="50" t="s">
+      <c r="B48" s="44" t="s">
         <v>299</v>
       </c>
       <c r="C48" t="s">
@@ -39627,7 +39627,7 @@
       <c r="A49" t="s">
         <v>301</v>
       </c>
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="44" t="s">
         <v>302</v>
       </c>
       <c r="C49" t="s">
@@ -39737,7 +39737,7 @@
       <c r="A50" t="s">
         <v>304</v>
       </c>
-      <c r="B50" s="50" t="s">
+      <c r="B50" s="44" t="s">
         <v>305</v>
       </c>
       <c r="C50" t="s">
@@ -39855,7 +39855,7 @@
       <c r="A52" t="s">
         <v>307</v>
       </c>
-      <c r="B52" s="50" t="s">
+      <c r="B52" s="44" t="s">
         <v>308</v>
       </c>
       <c r="C52" t="s">
@@ -39965,7 +39965,7 @@
       <c r="A53" t="s">
         <v>295</v>
       </c>
-      <c r="B53" s="50" t="s">
+      <c r="B53" s="44" t="s">
         <v>310</v>
       </c>
       <c r="C53" t="s">
@@ -40075,7 +40075,7 @@
       <c r="A54" t="s">
         <v>311</v>
       </c>
-      <c r="B54" s="50" t="s">
+      <c r="B54" s="44" t="s">
         <v>312</v>
       </c>
       <c r="C54" t="s">
@@ -40185,7 +40185,7 @@
       <c r="A55" t="s">
         <v>314</v>
       </c>
-      <c r="B55" s="50" t="s">
+      <c r="B55" s="44" t="s">
         <v>315</v>
       </c>
       <c r="C55" t="s">
@@ -40295,7 +40295,7 @@
       <c r="A56" t="s">
         <v>316</v>
       </c>
-      <c r="B56" s="50" t="s">
+      <c r="B56" s="44" t="s">
         <v>317</v>
       </c>
       <c r="C56" t="s">
@@ -40413,7 +40413,7 @@
       <c r="A58" t="s">
         <v>319</v>
       </c>
-      <c r="B58" s="50" t="s">
+      <c r="B58" s="44" t="s">
         <v>320</v>
       </c>
       <c r="C58" t="s">
@@ -40523,7 +40523,7 @@
       <c r="A59" t="s">
         <v>322</v>
       </c>
-      <c r="B59" s="50" t="s">
+      <c r="B59" s="44" t="s">
         <v>323</v>
       </c>
       <c r="C59" t="s">
@@ -40633,7 +40633,7 @@
       <c r="A60" t="s">
         <v>324</v>
       </c>
-      <c r="B60" s="50" t="s">
+      <c r="B60" s="44" t="s">
         <v>325</v>
       </c>
       <c r="C60" t="s">
@@ -40743,7 +40743,7 @@
       <c r="A61" t="s">
         <v>326</v>
       </c>
-      <c r="B61" s="50" t="s">
+      <c r="B61" s="44" t="s">
         <v>327</v>
       </c>
       <c r="C61" t="s">
@@ -40861,7 +40861,7 @@
       <c r="A63" t="s">
         <v>288</v>
       </c>
-      <c r="B63" s="50" t="s">
+      <c r="B63" s="44" t="s">
         <v>329</v>
       </c>
       <c r="C63" t="s">
@@ -40971,7 +40971,7 @@
       <c r="A64" t="s">
         <v>290</v>
       </c>
-      <c r="B64" s="50" t="s">
+      <c r="B64" s="44" t="s">
         <v>331</v>
       </c>
       <c r="C64" t="s">
@@ -41097,7 +41097,7 @@
       <c r="A67" t="s">
         <v>334</v>
       </c>
-      <c r="B67" s="50" t="s">
+      <c r="B67" s="44" t="s">
         <v>335</v>
       </c>
       <c r="C67" t="s">
@@ -41207,7 +41207,7 @@
       <c r="A68" t="s">
         <v>337</v>
       </c>
-      <c r="B68" s="50" t="s">
+      <c r="B68" s="44" t="s">
         <v>338</v>
       </c>
       <c r="C68" t="s">
@@ -41317,7 +41317,7 @@
       <c r="A69" t="s">
         <v>339</v>
       </c>
-      <c r="B69" s="50" t="s">
+      <c r="B69" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C69" t="s">
@@ -41435,7 +41435,7 @@
       <c r="A71" t="s">
         <v>334</v>
       </c>
-      <c r="B71" s="50" t="s">
+      <c r="B71" s="44" t="s">
         <v>341</v>
       </c>
       <c r="C71" t="s">
@@ -41545,7 +41545,7 @@
       <c r="A72" t="s">
         <v>337</v>
       </c>
-      <c r="B72" s="50" t="s">
+      <c r="B72" s="44" t="s">
         <v>342</v>
       </c>
       <c r="C72" t="s">
@@ -41655,7 +41655,7 @@
       <c r="A73" t="s">
         <v>339</v>
       </c>
-      <c r="B73" s="50" t="s">
+      <c r="B73" s="44" t="s">
         <v>343</v>
       </c>
       <c r="C73" t="s">
@@ -41789,7 +41789,7 @@
       <c r="A77" t="s">
         <v>346</v>
       </c>
-      <c r="B77" s="50" t="s">
+      <c r="B77" s="44" t="s">
         <v>347</v>
       </c>
       <c r="C77" t="s">
@@ -41899,7 +41899,7 @@
       <c r="A78" t="s">
         <v>349</v>
       </c>
-      <c r="B78" s="50" t="s">
+      <c r="B78" s="44" t="s">
         <v>350</v>
       </c>
       <c r="C78" t="s">
@@ -42009,7 +42009,7 @@
       <c r="A79" t="s">
         <v>351</v>
       </c>
-      <c r="B79" s="50" t="s">
+      <c r="B79" s="44" t="s">
         <v>352</v>
       </c>
       <c r="C79" t="s">
@@ -42119,7 +42119,7 @@
       <c r="A80" t="s">
         <v>257</v>
       </c>
-      <c r="B80" s="50" t="s">
+      <c r="B80" s="44" t="s">
         <v>353</v>
       </c>
       <c r="C80" t="s">
@@ -42237,7 +42237,7 @@
       <c r="A82" t="s">
         <v>346</v>
       </c>
-      <c r="B82" s="50" t="s">
+      <c r="B82" s="44" t="s">
         <v>354</v>
       </c>
       <c r="C82" t="s">
@@ -42347,7 +42347,7 @@
       <c r="A83" t="s">
         <v>349</v>
       </c>
-      <c r="B83" s="50" t="s">
+      <c r="B83" s="44" t="s">
         <v>356</v>
       </c>
       <c r="C83" t="s">
@@ -42457,7 +42457,7 @@
       <c r="A84" t="s">
         <v>351</v>
       </c>
-      <c r="B84" s="50" t="s">
+      <c r="B84" s="44" t="s">
         <v>357</v>
       </c>
       <c r="C84" t="s">
@@ -42567,7 +42567,7 @@
       <c r="A85" t="s">
         <v>257</v>
       </c>
-      <c r="B85" s="50" t="s">
+      <c r="B85" s="44" t="s">
         <v>358</v>
       </c>
       <c r="C85" t="s">
@@ -42685,7 +42685,7 @@
       <c r="A87" t="s">
         <v>360</v>
       </c>
-      <c r="B87" s="50" t="s">
+      <c r="B87" s="44" t="s">
         <v>361</v>
       </c>
       <c r="C87" t="s">
@@ -42795,7 +42795,7 @@
       <c r="A88" t="s">
         <v>362</v>
       </c>
-      <c r="B88" s="50" t="s">
+      <c r="B88" s="44" t="s">
         <v>363</v>
       </c>
       <c r="C88" t="s">
@@ -42913,7 +42913,7 @@
       <c r="A90" t="s">
         <v>346</v>
       </c>
-      <c r="B90" s="50" t="s">
+      <c r="B90" s="44" t="s">
         <v>365</v>
       </c>
       <c r="C90" t="s">
@@ -43023,7 +43023,7 @@
       <c r="A91" t="s">
         <v>349</v>
       </c>
-      <c r="B91" s="50" t="s">
+      <c r="B91" s="44" t="s">
         <v>367</v>
       </c>
       <c r="C91" t="s">
@@ -43133,7 +43133,7 @@
       <c r="A92" t="s">
         <v>351</v>
       </c>
-      <c r="B92" s="50" t="s">
+      <c r="B92" s="44" t="s">
         <v>368</v>
       </c>
       <c r="C92" t="s">
@@ -43243,7 +43243,7 @@
       <c r="A93" t="s">
         <v>257</v>
       </c>
-      <c r="B93" s="50" t="s">
+      <c r="B93" s="44" t="s">
         <v>369</v>
       </c>
       <c r="C93" t="s">
@@ -43359,11 +43359,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D8A44D-88EA-40FD-9C09-502A5C75600E}">
   <dimension ref="A1:AK81"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="35.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -49940,37 +49943,37 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
     </row>
     <row r="3" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48"/>
     </row>
     <row r="4" spans="1:7" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
     </row>
     <row r="5" spans="1:7" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
@@ -55017,15 +55020,15 @@
       <c r="G224" s="27"/>
     </row>
     <row r="225" spans="1:7" s="20" customFormat="1" ht="206.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="49" t="s">
+      <c r="A225" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="B225" s="49"/>
-      <c r="C225" s="49"/>
-      <c r="D225" s="49"/>
-      <c r="E225" s="49"/>
-      <c r="F225" s="49"/>
-      <c r="G225" s="49"/>
+      <c r="B225" s="50"/>
+      <c r="C225" s="50"/>
+      <c r="D225" s="50"/>
+      <c r="E225" s="50"/>
+      <c r="F225" s="50"/>
+      <c r="G225" s="50"/>
     </row>
     <row r="226" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226"/>
@@ -55062,8 +55065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA048DE0-AEAD-4096-B0F3-BDB0F419C9A6}">
   <dimension ref="A1:BD118"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57023,7 +57026,7 @@
       </c>
       <c r="D24" s="31"/>
       <c r="E24" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="31">
         <v>0</v>
@@ -67909,7 +67912,9 @@
   </sheetPr>
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -68028,7 +68033,7 @@
       </c>
       <c r="C2" s="31">
         <f>Calculations!E24</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="31">
         <f>Calculations!F24</f>

</xml_diff>